<commit_message>
updated to reflect revised staff count data from DCMS for Arts Council of England
</commit_message>
<xml_diff>
--- a/Data/2024-12-17 Public Bodies Directory 2022_23.xlsx
+++ b/Data/2024-12-17 Public Bodies Directory 2022_23.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2549" uniqueCount="2549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2551" uniqueCount="2551">
   <si>
     <t xml:space="preserve">Public Bodies Directory 2022/23</t>
   </si>
@@ -3269,7 +3269,7 @@
     <t xml:space="preserve">Office of Gas and Electricity Markets</t>
   </si>
   <si>
-    <t xml:space="preserve">PBTUID-5ac56f53-aac0-43b8-8a43-62af7aa277a1</t>
+    <t xml:space="preserve">PBTUID-2fc35ea0-9234-41d4-ad3c-2fe7f97e66c9</t>
   </si>
   <si>
     <t xml:space="preserve">OFGEM</t>
@@ -6107,7 +6107,7 @@
     <t xml:space="preserve">UK Infrastructure Bank Limited</t>
   </si>
   <si>
-    <t xml:space="preserve">PBTUID-a3167422-0794-4f50-989f-2d08a91802dc</t>
+    <t xml:space="preserve">PBTUID-99633933-ae75-42d9-8820-2172293040be</t>
   </si>
   <si>
     <t xml:space="preserve">UKIB</t>
@@ -7665,6 +7665,12 @@
   </si>
   <si>
     <t xml:space="preserve">Updated FTE in post value for Committee for Standards in Public Life (CO) to 5 FTE from originally 0 FTE.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025-02-24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updated FTE in post value for The Arts Council England (DCMS) from 643 to 601 FTE</t>
   </si>
 </sst>
 </file>
@@ -7925,7 +7931,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="revisions" displayName="revisions" ref="A5:B10" totalsRowCount="0" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="revisions" displayName="revisions" ref="A5:B11" totalsRowCount="0" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Date"/>
     <tableColumn id="2" name="Text"/>
@@ -8391,8 +8397,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
-    <col min="1" max="1" width="16.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="32.71" hidden="0" customWidth="1"/>
+    <col min="1" max="1" width="40.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="70.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="16.71" hidden="0" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8433,10 +8439,10 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="6" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -8444,10 +8450,10 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="6" t="s">
         <v>38</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -8455,10 +8461,10 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="6" t="s">
         <v>40</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -8466,10 +8472,10 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -8477,10 +8483,10 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="6" t="s">
         <v>44</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -8488,10 +8494,10 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="6" t="s">
         <v>47</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -8499,10 +8505,10 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="6" t="s">
         <v>49</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -8510,10 +8516,10 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="6" t="s">
         <v>51</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -8521,10 +8527,10 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="6" t="s">
         <v>53</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -8532,10 +8538,10 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="6" t="s">
         <v>55</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -8543,10 +8549,10 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="6" t="s">
         <v>57</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -8554,10 +8560,10 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="6" t="s">
         <v>59</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -8565,10 +8571,10 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="6" t="s">
         <v>62</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -8576,10 +8582,10 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="6" t="s">
         <v>64</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -8587,10 +8593,10 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="6" t="s">
         <v>66</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -8598,10 +8604,10 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="6" t="s">
         <v>68</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -8609,10 +8615,10 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="6" t="s">
         <v>70</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -8620,10 +8626,10 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="6" t="s">
         <v>72</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -8631,10 +8637,10 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="3" t="s">
+      <c r="A25" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="6" t="s">
         <v>74</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -8642,10 +8648,10 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="6" t="s">
         <v>77</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -8653,10 +8659,10 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="6" t="s">
         <v>79</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -8664,10 +8670,10 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="6" t="s">
         <v>81</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -8675,10 +8681,10 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="6" t="s">
         <v>83</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -8686,10 +8692,10 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="6" t="s">
         <v>85</v>
       </c>
       <c r="C30" s="3" t="s">
@@ -8697,10 +8703,10 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -8708,10 +8714,10 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="6" t="s">
         <v>90</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -8719,10 +8725,10 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="6" t="s">
         <v>92</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -8730,10 +8736,10 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="6" t="s">
         <v>94</v>
       </c>
       <c r="C34" s="3" t="s">
@@ -8741,10 +8747,10 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="6" t="s">
         <v>96</v>
       </c>
       <c r="C35" s="3" t="s">
@@ -8752,10 +8758,10 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="6" t="s">
         <v>98</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -8763,10 +8769,10 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="6" t="s">
         <v>100</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -8774,10 +8780,10 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="6" t="s">
         <v>102</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -8785,10 +8791,10 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="6" t="s">
         <v>105</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -8796,10 +8802,10 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="6" t="s">
         <v>107</v>
       </c>
       <c r="C40" s="3" t="s">
@@ -8807,10 +8813,10 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="6" t="s">
         <v>109</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -8818,10 +8824,10 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="6" t="s">
         <v>111</v>
       </c>
       <c r="C42" s="3" t="s">
@@ -8829,10 +8835,10 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="6" t="s">
         <v>113</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -8840,10 +8846,10 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="6" t="s">
         <v>115</v>
       </c>
       <c r="C44" s="3" t="s">
@@ -8851,10 +8857,10 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="6" t="s">
         <v>117</v>
       </c>
       <c r="C45" s="3" t="s">
@@ -8862,10 +8868,10 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="6" t="s">
         <v>119</v>
       </c>
       <c r="C46" s="3" t="s">
@@ -8873,10 +8879,10 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="6" t="s">
         <v>121</v>
       </c>
       <c r="C47" s="3" t="s">
@@ -8884,10 +8890,10 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="3" t="s">
+      <c r="A48" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="6" t="s">
         <v>123</v>
       </c>
       <c r="C48" s="3" t="s">
@@ -8895,10 +8901,10 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="6" t="s">
         <v>125</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -8906,10 +8912,10 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="6" t="s">
         <v>127</v>
       </c>
       <c r="C50" s="3" t="s">
@@ -8917,10 +8923,10 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C51" s="3" t="s">
@@ -8928,10 +8934,10 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="6" t="s">
         <v>131</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -8939,10 +8945,10 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="6" t="s">
         <v>133</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -8950,10 +8956,10 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C54" s="3" t="s">
@@ -8961,10 +8967,10 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="3" t="s">
+      <c r="A55" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="6" t="s">
         <v>137</v>
       </c>
       <c r="C55" s="3" t="s">
@@ -8972,10 +8978,10 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="3" t="s">
+      <c r="A56" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="6" t="s">
         <v>139</v>
       </c>
       <c r="C56" s="3" t="s">
@@ -8983,10 +8989,10 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="6" t="s">
         <v>141</v>
       </c>
       <c r="C57" s="3" t="s">
@@ -8994,15 +9000,23 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="6" t="s">
         <v>143</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>36</v>
       </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="6"/>
+      <c r="B59" s="6"/>
+    </row>
+    <row r="60">
+      <c r="A60" s="6"/>
+      <c r="B60" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9022,7 +9036,7 @@
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
     <col min="1" max="1" width="16.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="16.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="30.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="30.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="30.71" hidden="0" customWidth="1"/>
     <col min="5" max="5" width="30.71" hidden="0" customWidth="1"/>
@@ -9104,7 +9118,7 @@
         <v>305</v>
       </c>
       <c r="D6" s="13" t="n">
-        <v>390849.86</v>
+        <v>390807.86</v>
       </c>
       <c r="E6" s="14" t="n">
         <v>353296995790.17</v>
@@ -9256,7 +9270,7 @@
         <v>118</v>
       </c>
       <c r="D10" s="13" t="n">
-        <v>148086.25</v>
+        <v>148044.25</v>
       </c>
       <c r="E10" s="14" t="n">
         <v>217349604397.11</v>
@@ -9360,6 +9374,7 @@
       </c>
     </row>
     <row r="13">
+      <c r="B13" s="10"/>
       <c r="C13" s="12"/>
       <c r="D13" s="13"/>
       <c r="E13" s="14"/>
@@ -9372,6 +9387,7 @@
       <c r="L13" s="21"/>
     </row>
     <row r="14">
+      <c r="B14" s="10"/>
       <c r="C14" s="12"/>
       <c r="D14" s="13"/>
       <c r="E14" s="14"/>
@@ -9401,7 +9417,7 @@
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <cols>
     <col min="1" max="1" width="16.71" hidden="0" customWidth="1"/>
-    <col min="2" max="2" width="32.71" hidden="0" customWidth="1"/>
+    <col min="2" max="2" width="50.71" hidden="0" customWidth="1"/>
     <col min="3" max="3" width="30.71" hidden="0" customWidth="1"/>
     <col min="4" max="4" width="30.71" hidden="0" customWidth="1"/>
     <col min="5" max="5" width="30.71" hidden="0" customWidth="1"/>
@@ -9483,7 +9499,7 @@
         <v>305</v>
       </c>
       <c r="D6" s="23" t="n">
-        <v>390849.86</v>
+        <v>390807.86</v>
       </c>
       <c r="E6" s="24" t="n">
         <v>353296995790.17</v>
@@ -9635,7 +9651,7 @@
         <v>36</v>
       </c>
       <c r="D10" s="23" t="n">
-        <v>14150.07</v>
+        <v>14108.07</v>
       </c>
       <c r="E10" s="24" t="n">
         <v>2254292000</v>
@@ -10385,6 +10401,7 @@
       </c>
     </row>
     <row r="30">
+      <c r="B30" s="10"/>
       <c r="C30" s="22"/>
       <c r="D30" s="23"/>
       <c r="E30" s="24"/>
@@ -10397,6 +10414,7 @@
       <c r="L30" s="31"/>
     </row>
     <row r="31">
+      <c r="B31" s="10"/>
       <c r="C31" s="22"/>
       <c r="D31" s="23"/>
       <c r="E31" s="24"/>
@@ -19210,7 +19228,7 @@
         <v>204</v>
       </c>
       <c r="AI63" s="10" t="n">
-        <v>643</v>
+        <v>601</v>
       </c>
       <c r="AJ63" s="3" t="s">
         <v>291</v>
@@ -50345,6 +50363,14 @@
         <v>2548</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" s="3" t="s">
+        <v>2549</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>2550</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>